<commit_message>
rather than requiring the user to ensure invigilator timeslot availability doesnt contain 2 consectuive timeslots in a day, this is added as a constraint, also the fill colour for the excel output has been fixed (the last exam had no colour assigned to it)
</commit_message>
<xml_diff>
--- a/attempt2/invigilator_assignments.xlsx
+++ b/attempt2/invigilator_assignments.xlsx
@@ -29,7 +29,7 @@
       <color rgb="00FFFFFF"/>
     </font>
   </fonts>
-  <fills count="75">
+  <fills count="77">
     <fill>
       <patternFill/>
     </fill>
@@ -38,440 +38,452 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0075b3ef"/>
-        <bgColor rgb="0075b3ef"/>
+        <fgColor rgb="00c9ea47"/>
+        <bgColor rgb="00c9ea47"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0075efa9"/>
-        <bgColor rgb="0075efa9"/>
+        <fgColor rgb="00ea475e"/>
+        <bgColor rgb="00ea475e"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0075efd8"/>
-        <bgColor rgb="0075efd8"/>
+        <fgColor rgb="0047ea88"/>
+        <bgColor rgb="0047ea88"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0075d8ef"/>
-        <bgColor rgb="0075d8ef"/>
+        <fgColor rgb="0056ea47"/>
+        <bgColor rgb="0056ea47"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0075ef8e"/>
-        <bgColor rgb="0075ef8e"/>
+        <fgColor rgb="00a7ea47"/>
+        <bgColor rgb="00a7ea47"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00ef7591"/>
-        <bgColor rgb="00ef7591"/>
+        <fgColor rgb="006dea47"/>
+        <bgColor rgb="006dea47"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="007584ef"/>
-        <bgColor rgb="007584ef"/>
+        <fgColor rgb="0047abea"/>
+        <bgColor rgb="0047abea"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00ef7e75"/>
-        <bgColor rgb="00ef7e75"/>
+        <fgColor rgb="0084ea47"/>
+        <bgColor rgb="0084ea47"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00e775ef"/>
-        <bgColor rgb="00e775ef"/>
+        <fgColor rgb="0062ea47"/>
+        <bgColor rgb="0062ea47"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00ef8775"/>
-        <bgColor rgb="00ef8775"/>
+        <fgColor rgb="00ea9847"/>
+        <bgColor rgb="00ea9847"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00efee75"/>
-        <bgColor rgb="00efee75"/>
+        <fgColor rgb="00ea4752"/>
+        <bgColor rgb="00ea4752"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00ef9a75"/>
-        <bgColor rgb="00ef9a75"/>
+        <fgColor rgb="005647ea"/>
+        <bgColor rgb="005647ea"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00deef75"/>
-        <bgColor rgb="00deef75"/>
+        <fgColor rgb="004794ea"/>
+        <bgColor rgb="004794ea"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0081ef75"/>
-        <bgColor rgb="0081ef75"/>
+        <fgColor rgb="00eadd47"/>
+        <bgColor rgb="00eadd47"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="008aef75"/>
-        <bgColor rgb="008aef75"/>
+        <fgColor rgb="0047ea9f"/>
+        <bgColor rgb="0047ea9f"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0094ef75"/>
-        <bgColor rgb="0094ef75"/>
+        <fgColor rgb="0047ea5a"/>
+        <bgColor rgb="0047ea5a"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00757bef"/>
-        <bgColor rgb="00757bef"/>
+        <fgColor rgb="0047eacd"/>
+        <bgColor rgb="0047eacd"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0075efcf"/>
-        <bgColor rgb="0075efcf"/>
+        <fgColor rgb="004766ea"/>
+        <bgColor rgb="004766ea"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00ef75d2"/>
-        <bgColor rgb="00ef75d2"/>
+        <fgColor rgb="00477dea"/>
+        <bgColor rgb="00477dea"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00b0ef75"/>
-        <bgColor rgb="00b0ef75"/>
+        <fgColor rgb="00ea5e47"/>
+        <bgColor rgb="00ea5e47"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00b975ef"/>
-        <bgColor rgb="00b975ef"/>
+        <fgColor rgb="00ea5247"/>
+        <bgColor rgb="00ea5247"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00a675ef"/>
-        <bgColor rgb="00a675ef"/>
+        <fgColor rgb="00ea8147"/>
+        <bgColor rgb="00ea8147"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="009d75ef"/>
-        <bgColor rgb="009d75ef"/>
+        <fgColor rgb="00ea47a3"/>
+        <bgColor rgb="00ea47a3"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00efbf75"/>
-        <bgColor rgb="00efbf75"/>
+        <fgColor rgb="00eaaf47"/>
+        <bgColor rgb="00eaaf47"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00ef757e"/>
-        <bgColor rgb="00ef757e"/>
+        <fgColor rgb="00474fea"/>
+        <bgColor rgb="00474fea"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00d5ef75"/>
-        <bgColor rgb="00d5ef75"/>
+        <fgColor rgb="0079ea47"/>
+        <bgColor rgb="0079ea47"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00758eef"/>
-        <bgColor rgb="00758eef"/>
+        <fgColor rgb="00ea47af"/>
+        <bgColor rgb="00ea47af"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0075c5ef"/>
-        <bgColor rgb="0075c5ef"/>
+        <fgColor rgb="0047ea7d"/>
+        <bgColor rgb="0047ea7d"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00ef75a3"/>
-        <bgColor rgb="00ef75a3"/>
+        <fgColor rgb="00ea4780"/>
+        <bgColor rgb="00ea4780"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00efdb75"/>
-        <bgColor rgb="00efdb75"/>
+        <fgColor rgb="009047ea"/>
+        <bgColor rgb="009047ea"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00ef75bf"/>
-        <bgColor rgb="00ef75bf"/>
+        <fgColor rgb="00ea47e8"/>
+        <bgColor rgb="00ea47e8"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00efc875"/>
-        <bgColor rgb="00efc875"/>
+        <fgColor rgb="00ea47ba"/>
+        <bgColor rgb="00ea47ba"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0075efe1"/>
-        <bgColor rgb="0075efe1"/>
+        <fgColor rgb="0090ea47"/>
+        <bgColor rgb="0090ea47"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00efb675"/>
-        <bgColor rgb="00efb675"/>
+        <fgColor rgb="00ea4769"/>
+        <bgColor rgb="00ea4769"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00cc75ef"/>
-        <bgColor rgb="00cc75ef"/>
+        <fgColor rgb="00ea47c6"/>
+        <bgColor rgb="00ea47c6"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00efd275"/>
-        <bgColor rgb="00efd275"/>
+        <fgColor rgb="00b2ea47"/>
+        <bgColor rgb="00b2ea47"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="009def75"/>
-        <bgColor rgb="009def75"/>
+        <fgColor rgb="004788ea"/>
+        <bgColor rgb="004788ea"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00d575ef"/>
-        <bgColor rgb="00d575ef"/>
+        <fgColor rgb="004771ea"/>
+        <bgColor rgb="004771ea"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0078ef75"/>
-        <bgColor rgb="0078ef75"/>
+        <fgColor rgb="008447ea"/>
+        <bgColor rgb="008447ea"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00ef75db"/>
-        <bgColor rgb="00ef75db"/>
+        <fgColor rgb="00ea4798"/>
+        <bgColor rgb="00ea4798"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00efe475"/>
-        <bgColor rgb="00efe475"/>
+        <fgColor rgb="009b47ea"/>
+        <bgColor rgb="009b47ea"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0075efc5"/>
-        <bgColor rgb="0075efc5"/>
+        <fgColor rgb="0047d9ea"/>
+        <bgColor rgb="0047d9ea"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0075ef7b"/>
-        <bgColor rgb="0075ef7b"/>
+        <fgColor rgb="0047ea4f"/>
+        <bgColor rgb="0047ea4f"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00c2ef75"/>
-        <bgColor rgb="00c2ef75"/>
+        <fgColor rgb="00e047ea"/>
+        <bgColor rgb="00e047ea"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00efa375"/>
-        <bgColor rgb="00efa375"/>
+        <fgColor rgb="004b47ea"/>
+        <bgColor rgb="004b47ea"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0075ef84"/>
-        <bgColor rgb="0075ef84"/>
+        <fgColor rgb="006d47ea"/>
+        <bgColor rgb="006d47ea"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00ef75b6"/>
-        <bgColor rgb="00ef75b6"/>
+        <fgColor rgb="0047b6ea"/>
+        <bgColor rgb="0047b6ea"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0075a9ef"/>
-        <bgColor rgb="0075a9ef"/>
+        <fgColor rgb="0047eac2"/>
+        <bgColor rgb="0047eac2"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00ef7587"/>
-        <bgColor rgb="00ef7587"/>
+        <fgColor rgb="00a747ea"/>
+        <bgColor rgb="00a747ea"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00a6ef75"/>
-        <bgColor rgb="00a6ef75"/>
+        <fgColor rgb="0047eab6"/>
+        <bgColor rgb="0047eab6"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="009475ef"/>
-        <bgColor rgb="009475ef"/>
+        <fgColor rgb="00ea6947"/>
+        <bgColor rgb="00ea6947"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0075cfef"/>
-        <bgColor rgb="0075cfef"/>
+        <fgColor rgb="006247ea"/>
+        <bgColor rgb="006247ea"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00ccef75"/>
-        <bgColor rgb="00ccef75"/>
+        <fgColor rgb="00ea7547"/>
+        <bgColor rgb="00ea7547"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0075efbc"/>
-        <bgColor rgb="0075efbc"/>
+        <fgColor rgb="00e1ea47"/>
+        <bgColor rgb="00e1ea47"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0075efa0"/>
-        <bgColor rgb="0075efa0"/>
+        <fgColor rgb="0047ea71"/>
+        <bgColor rgb="0047ea71"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00ef9175"/>
-        <bgColor rgb="00ef9175"/>
+        <fgColor rgb="004bea47"/>
+        <bgColor rgb="004bea47"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00ef759a"/>
-        <bgColor rgb="00ef759a"/>
+        <fgColor rgb="00beea47"/>
+        <bgColor rgb="00beea47"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0075ef97"/>
-        <bgColor rgb="0075ef97"/>
+        <fgColor rgb="0047ea94"/>
+        <bgColor rgb="0047ea94"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00b075ef"/>
-        <bgColor rgb="00b075ef"/>
+        <fgColor rgb="00d5ea47"/>
+        <bgColor rgb="00d5ea47"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00de75ef"/>
-        <bgColor rgb="00de75ef"/>
+        <fgColor rgb="00eaa347"/>
+        <bgColor rgb="00eaa347"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00e7ef75"/>
-        <bgColor rgb="00e7ef75"/>
+        <fgColor rgb="00b247ea"/>
+        <bgColor rgb="00b247ea"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0075efeb"/>
-        <bgColor rgb="0075efeb"/>
+        <fgColor rgb="00ea4775"/>
+        <bgColor rgb="00ea4775"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0075ebef"/>
-        <bgColor rgb="0075ebef"/>
+        <fgColor rgb="00d547ea"/>
+        <bgColor rgb="00d547ea"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00b9ef75"/>
-        <bgColor rgb="00b9ef75"/>
+        <fgColor rgb="00eaba47"/>
+        <bgColor rgb="00eaba47"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0075bcef"/>
-        <bgColor rgb="0075bcef"/>
+        <fgColor rgb="00eae847"/>
+        <bgColor rgb="00eae847"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00efad75"/>
-        <bgColor rgb="00efad75"/>
+        <fgColor rgb="00ea47dd"/>
+        <bgColor rgb="00ea47dd"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00ef75ee"/>
-        <bgColor rgb="00ef75ee"/>
+        <fgColor rgb="0047c2ea"/>
+        <bgColor rgb="0047c2ea"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="008175ef"/>
-        <bgColor rgb="008175ef"/>
+        <fgColor rgb="009bea47"/>
+        <bgColor rgb="009bea47"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="007875ef"/>
-        <bgColor rgb="007875ef"/>
+        <fgColor rgb="00eac647"/>
+        <bgColor rgb="00eac647"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00ef75c8"/>
-        <bgColor rgb="00ef75c8"/>
+        <fgColor rgb="00c947ea"/>
+        <bgColor rgb="00c947ea"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0075efb3"/>
-        <bgColor rgb="0075efb3"/>
+        <fgColor rgb="00ead147"/>
+        <bgColor rgb="00ead147"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0075a0ef"/>
-        <bgColor rgb="0075a0ef"/>
+        <fgColor rgb="0047ead9"/>
+        <bgColor rgb="0047ead9"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0075e1ef"/>
-        <bgColor rgb="0075e1ef"/>
+        <fgColor rgb="0047eae4"/>
+        <bgColor rgb="0047eae4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00ea8c47"/>
+        <bgColor rgb="00ea8c47"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0047cdea"/>
+        <bgColor rgb="0047cdea"/>
       </patternFill>
     </fill>
   </fills>
@@ -487,17 +499,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -505,97 +517,116 @@
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="22" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="23" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="24" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="25" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="26" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="29" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="30" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="34" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="35" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="36" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="37" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="41" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="42" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="38" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="39" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="40" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="41" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="42" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="43" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="44" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="36" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="45" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="46" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="47" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="48" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="49" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="40" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="50" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="51" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="52" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="52" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="53" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="51" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="45" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="54" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="55" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="56" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="37" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="57" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="56" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="57" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="53" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="58" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="59" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="60" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="61" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="62" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="62" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="63" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="60" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="54" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="45" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="61" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="64" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="65" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="50" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="65" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="66" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="67" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="65" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="68" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="69" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="70" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="70" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="71" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="63" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="72" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="73" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="71" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="74" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="54" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="39" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="57" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="66" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="42" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="56" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="51" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="75" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="76" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="33" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="72" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="76" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="46" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="52" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="56" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="49" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="64" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="58" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -1087,9 +1118,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="E2" s="1" t="inlineStr">
+        <is>
+          <t>Exam17</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -1097,9 +1128,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="G2" s="2" t="inlineStr">
+        <is>
+          <t>Exam28</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -1184,9 +1215,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="E3" s="3" t="inlineStr">
+        <is>
+          <t>Exam17</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -1199,7 +1230,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="H3" s="1" t="inlineStr">
+      <c r="H3" s="4" t="inlineStr">
         <is>
           <t>Exam34</t>
         </is>
@@ -1214,9 +1245,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="K3" s="5" t="inlineStr">
+        <is>
+          <t>Exam47</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
@@ -1229,9 +1260,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="N3" s="2" t="inlineStr">
-        <is>
-          <t>Exam58</t>
+      <c r="N3" s="6" t="inlineStr">
+        <is>
+          <t>Exam60</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
@@ -1244,9 +1275,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="Q3" s="3" t="inlineStr">
-        <is>
-          <t>Exam72</t>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
@@ -1254,9 +1285,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>Exam74</t>
+      <c r="S3" s="7" t="inlineStr">
+        <is>
+          <t>Exam75</t>
         </is>
       </c>
     </row>
@@ -1271,9 +1302,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="C4" s="4" t="inlineStr">
-        <is>
-          <t>Exam7</t>
+      <c r="C4" s="8" t="inlineStr">
+        <is>
+          <t>Exam8</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1281,7 +1312,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="E4" s="5" t="inlineStr">
+      <c r="E4" s="9" t="inlineStr">
         <is>
           <t>Exam18</t>
         </is>
@@ -1296,14 +1327,14 @@
           <t>-</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I4" s="6" t="inlineStr">
-        <is>
-          <t>Exam39</t>
+      <c r="H4" s="4" t="inlineStr">
+        <is>
+          <t>Exam34</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -1311,9 +1342,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="K4" s="7" t="inlineStr">
-        <is>
-          <t>Exam48</t>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
@@ -1331,9 +1362,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="O4" s="8" t="inlineStr">
-        <is>
-          <t>Exam66</t>
+      <c r="O4" s="10" t="inlineStr">
+        <is>
+          <t>Exam61</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
@@ -1351,9 +1382,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="S4" s="9" t="inlineStr">
-        <is>
-          <t>Exam74</t>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
     </row>
@@ -1383,9 +1414,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="F5" s="10" t="inlineStr">
-        <is>
-          <t>Exam24</t>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -1393,9 +1424,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="H5" s="4" t="inlineStr">
+        <is>
+          <t>Exam34</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -1413,9 +1444,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="L5" s="11" t="inlineStr">
-        <is>
-          <t>Exam53</t>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
@@ -1433,9 +1464,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="P5" s="12" t="inlineStr">
-        <is>
-          <t>Exam68</t>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
@@ -1448,9 +1479,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="S5" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="S5" s="11" t="inlineStr">
+        <is>
+          <t>Exam72</t>
         </is>
       </c>
     </row>
@@ -1470,9 +1501,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="D6" s="12" t="inlineStr">
+        <is>
+          <t>Exam14</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -1485,9 +1516,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="G6" s="13" t="inlineStr">
-        <is>
-          <t>Exam27</t>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -1495,14 +1526,14 @@
           <t>-</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J6" s="14" t="inlineStr">
-        <is>
-          <t>Exam42</t>
+      <c r="I6" s="13" t="inlineStr">
+        <is>
+          <t>Exam38</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
@@ -1525,14 +1556,14 @@
           <t>-</t>
         </is>
       </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="P6" s="15" t="inlineStr">
-        <is>
-          <t>Exam70</t>
+      <c r="O6" s="14" t="inlineStr">
+        <is>
+          <t>Exam65</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
@@ -1545,9 +1576,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="S6" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="S6" s="15" t="inlineStr">
+        <is>
+          <t>Exam73</t>
         </is>
       </c>
     </row>
@@ -1557,9 +1588,9 @@
           <t>Amelia White</t>
         </is>
       </c>
-      <c r="B7" s="16" t="inlineStr">
-        <is>
-          <t>Exam4</t>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1572,9 +1603,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="E7" s="17" t="inlineStr">
-        <is>
-          <t>Exam17</t>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -1592,9 +1623,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="I7" s="18" t="inlineStr">
-        <is>
-          <t>Exam35</t>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
@@ -1659,7 +1690,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="C8" s="19" t="inlineStr">
+      <c r="C8" s="16" t="inlineStr">
         <is>
           <t>Exam6</t>
         </is>
@@ -1684,9 +1715,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="H8" s="17" t="inlineStr">
+        <is>
+          <t>Exam34</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -1751,9 +1782,9 @@
           <t>Andrew White</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="B9" s="18" t="inlineStr">
+        <is>
+          <t>Exam5</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -1781,14 +1812,14 @@
           <t>-</t>
         </is>
       </c>
-      <c r="H9" s="1" t="inlineStr">
-        <is>
-          <t>Exam34</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I9" s="19" t="inlineStr">
+        <is>
+          <t>Exam35</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
@@ -1796,9 +1827,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="K9" s="20" t="inlineStr">
-        <is>
-          <t>Exam51</t>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
@@ -1806,9 +1837,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="M9" s="21" t="inlineStr">
-        <is>
-          <t>Exam56</t>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
@@ -1836,9 +1867,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="S9" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="S9" s="20" t="inlineStr">
+        <is>
+          <t>Exam72</t>
         </is>
       </c>
     </row>
@@ -1853,9 +1884,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="C10" s="22" t="inlineStr">
-        <is>
-          <t>Exam10</t>
+      <c r="C10" s="21" t="inlineStr">
+        <is>
+          <t>Exam9</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -1883,9 +1914,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="I10" s="23" t="inlineStr">
-        <is>
-          <t>Exam36</t>
+      <c r="I10" s="22" t="inlineStr">
+        <is>
+          <t>Exam37</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
@@ -1893,14 +1924,14 @@
           <t>-</t>
         </is>
       </c>
-      <c r="K10" s="24" t="inlineStr">
-        <is>
-          <t>Exam49</t>
-        </is>
-      </c>
-      <c r="L10" s="25" t="inlineStr">
-        <is>
-          <t>Exam54</t>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
@@ -1908,9 +1939,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="N10" s="23" t="inlineStr">
+        <is>
+          <t>Exam57</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
@@ -1933,9 +1964,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="S10" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="S10" s="24" t="inlineStr">
+        <is>
+          <t>Exam71</t>
         </is>
       </c>
     </row>
@@ -1955,9 +1986,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="D11" s="26" t="inlineStr">
-        <is>
-          <t>Exam13</t>
+      <c r="D11" s="25" t="inlineStr">
+        <is>
+          <t>Exam15</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -1970,9 +2001,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="G11" s="27" t="inlineStr">
-        <is>
-          <t>Exam29</t>
+      <c r="G11" s="26" t="inlineStr">
+        <is>
+          <t>Exam27</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -1990,9 +2021,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="K11" s="28" t="inlineStr">
-        <is>
-          <t>Exam51</t>
+      <c r="K11" s="27" t="inlineStr">
+        <is>
+          <t>Exam44</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
@@ -2000,9 +2031,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="M11" s="29" t="inlineStr">
-        <is>
-          <t>Exam56</t>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
@@ -2010,9 +2041,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="O11" s="30" t="inlineStr">
-        <is>
-          <t>Exam61</t>
+      <c r="O11" s="28" t="inlineStr">
+        <is>
+          <t>Exam66</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
@@ -2020,9 +2051,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="Q11" s="31" t="inlineStr">
-        <is>
-          <t>Exam72</t>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
@@ -2030,9 +2061,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="S11" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="S11" s="7" t="inlineStr">
+        <is>
+          <t>Exam75</t>
         </is>
       </c>
     </row>
@@ -2052,9 +2083,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="D12" s="29" t="inlineStr">
+        <is>
+          <t>Exam15</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -2077,9 +2108,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="I12" s="18" t="inlineStr">
-        <is>
-          <t>Exam35</t>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
@@ -2107,7 +2138,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="O12" s="32" t="inlineStr">
+      <c r="O12" s="30" t="inlineStr">
         <is>
           <t>Exam66</t>
         </is>
@@ -2139,9 +2170,9 @@
           <t>Beatrice Lewis</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="B13" s="31" t="inlineStr">
+        <is>
+          <t>Exam4</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -2179,14 +2210,14 @@
           <t>-</t>
         </is>
       </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="J13" s="32" t="inlineStr">
+        <is>
+          <t>Exam41</t>
+        </is>
+      </c>
+      <c r="K13" s="33" t="inlineStr">
+        <is>
+          <t>Exam48</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
@@ -2209,9 +2240,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="P13" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="P13" s="34" t="inlineStr">
+        <is>
+          <t>Exam70</t>
         </is>
       </c>
       <c r="Q13" t="inlineStr">
@@ -2224,9 +2255,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="S13" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="S13" s="20" t="inlineStr">
+        <is>
+          <t>Exam72</t>
         </is>
       </c>
     </row>
@@ -2266,9 +2297,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="H14" s="1" t="inlineStr">
-        <is>
-          <t>Exam34</t>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -2286,9 +2317,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="L14" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="L14" s="35" t="inlineStr">
+        <is>
+          <t>Exam53</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
@@ -2296,14 +2327,14 @@
           <t>-</t>
         </is>
       </c>
-      <c r="N14" s="33" t="inlineStr">
-        <is>
-          <t>Exam60</t>
-        </is>
-      </c>
-      <c r="O14" s="34" t="inlineStr">
-        <is>
-          <t>Exam65</t>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O14" s="30" t="inlineStr">
+        <is>
+          <t>Exam66</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
@@ -2358,9 +2389,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="G15" s="36" t="inlineStr">
+        <is>
+          <t>Exam26</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -2368,9 +2399,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="I15" s="35" t="inlineStr">
-        <is>
-          <t>Exam39</t>
+      <c r="I15" s="19" t="inlineStr">
+        <is>
+          <t>Exam35</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
@@ -2388,9 +2419,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="M15" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="M15" s="37" t="inlineStr">
+        <is>
+          <t>Exam55</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
@@ -2398,9 +2429,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="O15" s="32" t="inlineStr">
-        <is>
-          <t>Exam66</t>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
@@ -2440,9 +2471,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="D16" s="36" t="inlineStr">
-        <is>
-          <t>Exam15</t>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -2450,9 +2481,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="F16" s="37" t="inlineStr">
-        <is>
-          <t>Exam25</t>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -2460,9 +2491,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="H16" s="38" t="inlineStr">
+        <is>
+          <t>Exam32</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -2470,9 +2501,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="J16" s="38" t="inlineStr">
-        <is>
-          <t>Exam41</t>
+      <c r="J16" s="39" t="inlineStr">
+        <is>
+          <t>Exam42</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
@@ -2490,9 +2521,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="N16" s="39" t="inlineStr">
-        <is>
-          <t>Exam59</t>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="O16" t="inlineStr">
@@ -2502,7 +2533,7 @@
       </c>
       <c r="P16" s="40" t="inlineStr">
         <is>
-          <t>Exam67</t>
+          <t>Exam69</t>
         </is>
       </c>
       <c r="Q16" t="inlineStr">
@@ -2515,7 +2546,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="S16" s="9" t="inlineStr">
+      <c r="S16" s="41" t="inlineStr">
         <is>
           <t>Exam74</t>
         </is>
@@ -2552,9 +2583,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="G17" s="2" t="inlineStr">
+        <is>
+          <t>Exam28</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
@@ -2572,9 +2603,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="K17" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="K17" s="42" t="inlineStr">
+        <is>
+          <t>Exam51</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
@@ -2592,9 +2623,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="O17" s="41" t="inlineStr">
-        <is>
-          <t>Exam63</t>
+      <c r="O17" s="30" t="inlineStr">
+        <is>
+          <t>Exam66</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
@@ -2644,9 +2675,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="F18" s="43" t="inlineStr">
+        <is>
+          <t>Exam23</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -2654,7 +2685,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="H18" s="1" t="inlineStr">
+      <c r="H18" s="17" t="inlineStr">
         <is>
           <t>Exam34</t>
         </is>
@@ -2689,9 +2720,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="O18" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="O18" s="30" t="inlineStr">
+        <is>
+          <t>Exam66</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
@@ -2709,9 +2740,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="S18" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="S18" s="44" t="inlineStr">
+        <is>
+          <t>Exam74</t>
         </is>
       </c>
     </row>
@@ -2746,9 +2777,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="G19" s="42" t="inlineStr">
-        <is>
-          <t>Exam28</t>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -2848,9 +2879,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="H20" s="1" t="inlineStr">
-        <is>
-          <t>Exam34</t>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -2888,9 +2919,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="P20" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="P20" s="45" t="inlineStr">
+        <is>
+          <t>Exam67</t>
         </is>
       </c>
       <c r="Q20" t="inlineStr">
@@ -2903,9 +2934,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="S20" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="S20" s="44" t="inlineStr">
+        <is>
+          <t>Exam74</t>
         </is>
       </c>
     </row>
@@ -2925,9 +2956,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="D21" s="46" t="inlineStr">
+        <is>
+          <t>Exam13</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -2940,9 +2971,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="G21" s="43" t="inlineStr">
-        <is>
-          <t>Exam30</t>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -2950,9 +2981,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="I21" s="47" t="inlineStr">
+        <is>
+          <t>Exam39</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
@@ -2960,9 +2991,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="K21" s="44" t="inlineStr">
-        <is>
-          <t>Exam50</t>
+      <c r="K21" s="48" t="inlineStr">
+        <is>
+          <t>Exam51</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
@@ -2975,12 +3006,12 @@
           <t>-</t>
         </is>
       </c>
-      <c r="N21" s="45" t="inlineStr">
-        <is>
-          <t>Exam57</t>
-        </is>
-      </c>
-      <c r="O21" s="46" t="inlineStr">
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O21" s="49" t="inlineStr">
         <is>
           <t>Exam64</t>
         </is>
@@ -2990,9 +3021,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="Q21" s="31" t="inlineStr">
-        <is>
-          <t>Exam72</t>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="R21" t="inlineStr">
@@ -3047,7 +3078,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="I22" s="18" t="inlineStr">
+      <c r="I22" s="19" t="inlineStr">
         <is>
           <t>Exam35</t>
         </is>
@@ -3082,9 +3113,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="P22" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="P22" s="45" t="inlineStr">
+        <is>
+          <t>Exam67</t>
         </is>
       </c>
       <c r="Q22" t="inlineStr">
@@ -3124,9 +3155,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="E23" s="1" t="inlineStr">
+        <is>
+          <t>Exam17</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -3169,9 +3200,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="N23" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="N23" s="50" t="inlineStr">
+        <is>
+          <t>Exam57</t>
         </is>
       </c>
       <c r="O23" t="inlineStr">
@@ -3179,9 +3210,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="P23" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="P23" s="45" t="inlineStr">
+        <is>
+          <t>Exam67</t>
         </is>
       </c>
       <c r="Q23" t="inlineStr">
@@ -3271,19 +3302,19 @@
           <t>-</t>
         </is>
       </c>
-      <c r="O24" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="P24" s="47" t="inlineStr">
-        <is>
-          <t>Exam67</t>
-        </is>
-      </c>
-      <c r="Q24" s="3" t="inlineStr">
-        <is>
-          <t>Exam72</t>
+      <c r="O24" s="30" t="inlineStr">
+        <is>
+          <t>Exam66</t>
+        </is>
+      </c>
+      <c r="P24" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Q24" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="R24" t="inlineStr">
@@ -3303,9 +3334,9 @@
           <t>Elizabeth Mitchell</t>
         </is>
       </c>
-      <c r="B25" s="48" t="inlineStr">
-        <is>
-          <t>Exam2</t>
+      <c r="B25" s="51" t="inlineStr">
+        <is>
+          <t>Exam4</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -3318,7 +3349,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="E25" s="49" t="inlineStr">
+      <c r="E25" s="52" t="inlineStr">
         <is>
           <t>Exam19</t>
         </is>
@@ -3343,9 +3374,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="J25" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="J25" s="53" t="inlineStr">
+        <is>
+          <t>Exam40</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
@@ -3353,9 +3384,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="L25" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="L25" s="54" t="inlineStr">
+        <is>
+          <t>Exam52</t>
         </is>
       </c>
       <c r="M25" t="inlineStr">
@@ -3373,9 +3404,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="P25" s="40" t="inlineStr">
-        <is>
-          <t>Exam67</t>
+      <c r="P25" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="Q25" t="inlineStr">
@@ -3388,7 +3419,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="S25" s="9" t="inlineStr">
+      <c r="S25" s="41" t="inlineStr">
         <is>
           <t>Exam74</t>
         </is>
@@ -3405,9 +3436,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="C26" s="55" t="inlineStr">
+        <is>
+          <t>Exam10</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -3420,9 +3451,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="F26" s="56" t="inlineStr">
+        <is>
+          <t>Exam22</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -3435,9 +3466,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="I26" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="I26" s="57" t="inlineStr">
+        <is>
+          <t>Exam35</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
@@ -3445,9 +3476,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="K26" s="50" t="inlineStr">
-        <is>
-          <t>Exam44</t>
+      <c r="K26" s="58" t="inlineStr">
+        <is>
+          <t>Exam49</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
@@ -3465,9 +3496,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="O26" s="51" t="inlineStr">
-        <is>
-          <t>Exam63</t>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
@@ -3485,7 +3516,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="S26" s="9" t="inlineStr">
+      <c r="S26" s="41" t="inlineStr">
         <is>
           <t>Exam74</t>
         </is>
@@ -3537,9 +3568,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="J27" s="38" t="inlineStr">
-        <is>
-          <t>Exam41</t>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
@@ -3557,9 +3588,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="N27" s="45" t="inlineStr">
-        <is>
-          <t>Exam57</t>
+      <c r="N27" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="O27" t="inlineStr">
@@ -3567,14 +3598,14 @@
           <t>-</t>
         </is>
       </c>
-      <c r="P27" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="Q27" s="31" t="inlineStr">
-        <is>
-          <t>Exam72</t>
+      <c r="P27" s="59" t="inlineStr">
+        <is>
+          <t>Exam67</t>
+        </is>
+      </c>
+      <c r="Q27" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="R27" t="inlineStr">
@@ -3582,7 +3613,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="S27" s="9" t="inlineStr">
+      <c r="S27" s="41" t="inlineStr">
         <is>
           <t>Exam74</t>
         </is>
@@ -3594,9 +3625,9 @@
           <t>Ethan Bailey</t>
         </is>
       </c>
-      <c r="B28" s="52" t="inlineStr">
-        <is>
-          <t>Exam3</t>
+      <c r="B28" s="60" t="inlineStr">
+        <is>
+          <t>Exam5</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -3604,9 +3635,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="D28" s="53" t="inlineStr">
-        <is>
-          <t>Exam14</t>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -3614,9 +3645,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="F28" s="61" t="inlineStr">
+        <is>
+          <t>Exam25</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
@@ -3624,9 +3655,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="H28" s="54" t="inlineStr">
-        <is>
-          <t>Exam31</t>
+      <c r="H28" s="4" t="inlineStr">
+        <is>
+          <t>Exam34</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
@@ -3634,9 +3665,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="J28" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="J28" s="62" t="inlineStr">
+        <is>
+          <t>Exam41</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
@@ -3659,9 +3690,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="O28" s="46" t="inlineStr">
-        <is>
-          <t>Exam64</t>
+      <c r="O28" s="63" t="inlineStr">
+        <is>
+          <t>Exam63</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
@@ -3669,9 +3700,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="Q28" s="31" t="inlineStr">
-        <is>
-          <t>Exam72</t>
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="R28" t="inlineStr">
@@ -3679,9 +3710,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="S28" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="S28" s="41" t="inlineStr">
+        <is>
+          <t>Exam74</t>
         </is>
       </c>
     </row>
@@ -3736,9 +3767,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="K29" s="20" t="inlineStr">
-        <is>
-          <t>Exam51</t>
+      <c r="K29" s="64" t="inlineStr">
+        <is>
+          <t>Exam43</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
@@ -3798,9 +3829,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="D30" s="55" t="inlineStr">
-        <is>
-          <t>Exam12</t>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -3808,9 +3839,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="F30" s="56" t="inlineStr">
-        <is>
-          <t>Exam21</t>
+      <c r="F30" s="65" t="inlineStr">
+        <is>
+          <t>Exam24</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
@@ -3818,7 +3849,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="H30" s="57" t="inlineStr">
+      <c r="H30" s="4" t="inlineStr">
         <is>
           <t>Exam34</t>
         </is>
@@ -3858,14 +3889,14 @@
           <t>-</t>
         </is>
       </c>
-      <c r="P30" s="40" t="inlineStr">
-        <is>
-          <t>Exam67</t>
-        </is>
-      </c>
-      <c r="Q30" s="31" t="inlineStr">
-        <is>
-          <t>Exam72</t>
+      <c r="P30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Q30" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="R30" t="inlineStr">
@@ -3873,9 +3904,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="S30" s="9" t="inlineStr">
-        <is>
-          <t>Exam74</t>
+      <c r="S30" s="15" t="inlineStr">
+        <is>
+          <t>Exam73</t>
         </is>
       </c>
     </row>
@@ -3885,9 +3916,9 @@
           <t>Frederick Bell</t>
         </is>
       </c>
-      <c r="B31" s="58" t="inlineStr">
-        <is>
-          <t>Exam4</t>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -3900,9 +3931,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="E31" s="59" t="inlineStr">
-        <is>
-          <t>Exam17</t>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -3910,9 +3941,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="G31" s="60" t="inlineStr">
-        <is>
-          <t>Exam26</t>
+      <c r="G31" s="66" t="inlineStr">
+        <is>
+          <t>Exam29</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
@@ -3920,9 +3951,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="I31" s="61" t="inlineStr">
-        <is>
-          <t>Exam35</t>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
@@ -3930,9 +3961,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="K31" s="62" t="inlineStr">
-        <is>
-          <t>Exam43</t>
+      <c r="K31" s="67" t="inlineStr">
+        <is>
+          <t>Exam45</t>
         </is>
       </c>
       <c r="L31" t="inlineStr">
@@ -3950,19 +3981,19 @@
           <t>-</t>
         </is>
       </c>
-      <c r="O31" s="63" t="inlineStr">
-        <is>
-          <t>Exam62</t>
-        </is>
-      </c>
-      <c r="P31" s="15" t="inlineStr">
-        <is>
-          <t>Exam70</t>
-        </is>
-      </c>
-      <c r="Q31" s="31" t="inlineStr">
-        <is>
-          <t>Exam72</t>
+      <c r="O31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Q31" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="R31" t="inlineStr">
@@ -3970,9 +4001,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="S31" s="64" t="inlineStr">
-        <is>
-          <t>Exam73</t>
+      <c r="S31" s="24" t="inlineStr">
+        <is>
+          <t>Exam71</t>
         </is>
       </c>
     </row>
@@ -4047,9 +4078,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="O32" s="32" t="inlineStr">
-        <is>
-          <t>Exam66</t>
+      <c r="O32" s="68" t="inlineStr">
+        <is>
+          <t>Exam62</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
@@ -4057,9 +4088,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="Q32" s="3" t="inlineStr">
-        <is>
-          <t>Exam72</t>
+      <c r="Q32" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="R32" t="inlineStr">
@@ -4104,9 +4135,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="G33" s="2" t="inlineStr">
+        <is>
+          <t>Exam28</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
@@ -4114,9 +4145,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="I33" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="I33" s="19" t="inlineStr">
+        <is>
+          <t>Exam35</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
@@ -4124,9 +4155,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="K33" s="65" t="inlineStr">
-        <is>
-          <t>Exam43</t>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="L33" t="inlineStr">
@@ -4149,7 +4180,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="P33" s="66" t="inlineStr">
+      <c r="P33" s="34" t="inlineStr">
         <is>
           <t>Exam70</t>
         </is>
@@ -4176,9 +4207,9 @@
           <t>Hannah Cooper</t>
         </is>
       </c>
-      <c r="B34" s="67" t="inlineStr">
-        <is>
-          <t>Exam3</t>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -4278,9 +4309,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="C35" s="19" t="inlineStr">
-        <is>
-          <t>Exam6</t>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -4303,9 +4334,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="H35" s="1" t="inlineStr">
-        <is>
-          <t>Exam34</t>
+      <c r="H35" s="69" t="inlineStr">
+        <is>
+          <t>Exam33</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
@@ -4313,9 +4344,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="J35" s="68" t="inlineStr">
-        <is>
-          <t>Exam42</t>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
@@ -4390,9 +4421,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="F36" s="70" t="inlineStr">
+        <is>
+          <t>Exam24</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
@@ -4405,9 +4436,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="I36" s="18" t="inlineStr">
-        <is>
-          <t>Exam35</t>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
@@ -4415,9 +4446,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="K36" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="K36" s="42" t="inlineStr">
+        <is>
+          <t>Exam51</t>
         </is>
       </c>
       <c r="L36" t="inlineStr">
@@ -4435,7 +4466,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="O36" s="32" t="inlineStr">
+      <c r="O36" s="30" t="inlineStr">
         <is>
           <t>Exam66</t>
         </is>
@@ -4467,9 +4498,9 @@
           <t>Isabella Ward</t>
         </is>
       </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="B37" s="71" t="inlineStr">
+        <is>
+          <t>Exam3</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -4482,9 +4513,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="E37" s="69" t="inlineStr">
-        <is>
-          <t>Exam16</t>
+      <c r="E37" s="72" t="inlineStr">
+        <is>
+          <t>Exam20</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -4497,9 +4528,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="H37" s="70" t="inlineStr">
-        <is>
-          <t>Exam32</t>
+      <c r="H37" s="73" t="inlineStr">
+        <is>
+          <t>Exam31</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
@@ -4527,9 +4558,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="N37" s="39" t="inlineStr">
-        <is>
-          <t>Exam59</t>
+      <c r="N37" s="74" t="inlineStr">
+        <is>
+          <t>Exam58</t>
         </is>
       </c>
       <c r="O37" t="inlineStr">
@@ -4542,9 +4573,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="Q37" s="71" t="inlineStr">
-        <is>
-          <t>Exam71</t>
+      <c r="Q37" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="R37" t="inlineStr">
@@ -4552,9 +4583,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="S37" s="64" t="inlineStr">
-        <is>
-          <t>Exam73</t>
+      <c r="S37" s="11" t="inlineStr">
+        <is>
+          <t>Exam72</t>
         </is>
       </c>
     </row>
@@ -4609,9 +4640,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="K38" s="20" t="inlineStr">
-        <is>
-          <t>Exam51</t>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="L38" t="inlineStr">
@@ -4629,14 +4660,14 @@
           <t>-</t>
         </is>
       </c>
-      <c r="O38" s="32" t="inlineStr">
-        <is>
-          <t>Exam66</t>
-        </is>
-      </c>
-      <c r="P38" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="O38" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P38" s="75" t="inlineStr">
+        <is>
+          <t>Exam69</t>
         </is>
       </c>
       <c r="Q38" t="inlineStr">
@@ -4671,9 +4702,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="D39" s="55" t="inlineStr">
-        <is>
-          <t>Exam12</t>
+      <c r="D39" s="76" t="inlineStr">
+        <is>
+          <t>Exam11</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -4686,7 +4717,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="G39" s="72" t="inlineStr">
+      <c r="G39" s="77" t="inlineStr">
         <is>
           <t>Exam28</t>
         </is>
@@ -4701,9 +4732,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="J39" s="73" t="inlineStr">
-        <is>
-          <t>Exam40</t>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
@@ -4711,9 +4742,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="L39" s="74" t="inlineStr">
-        <is>
-          <t>Exam52</t>
+      <c r="L39" s="78" t="inlineStr">
+        <is>
+          <t>Exam53</t>
         </is>
       </c>
       <c r="M39" t="inlineStr">
@@ -4731,9 +4762,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="P39" s="12" t="inlineStr">
-        <is>
-          <t>Exam68</t>
+      <c r="P39" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="Q39" t="inlineStr">
@@ -4746,9 +4777,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="S39" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="S39" s="11" t="inlineStr">
+        <is>
+          <t>Exam72</t>
         </is>
       </c>
     </row>
@@ -4758,9 +4789,9 @@
           <t>Jane Brooks</t>
         </is>
       </c>
-      <c r="B40" s="75" t="inlineStr">
-        <is>
-          <t>Exam5</t>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -4768,9 +4799,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="D40" s="12" t="inlineStr">
+        <is>
+          <t>Exam14</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
@@ -4778,9 +4809,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="F40" s="76" t="inlineStr">
-        <is>
-          <t>Exam23</t>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
@@ -4793,9 +4824,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="I40" s="77" t="inlineStr">
-        <is>
-          <t>Exam37</t>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
@@ -4803,9 +4834,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="K40" s="24" t="inlineStr">
-        <is>
-          <t>Exam49</t>
+      <c r="K40" s="79" t="inlineStr">
+        <is>
+          <t>Exam48</t>
         </is>
       </c>
       <c r="L40" t="inlineStr">
@@ -4813,9 +4844,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="M40" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="M40" s="80" t="inlineStr">
+        <is>
+          <t>Exam56</t>
         </is>
       </c>
       <c r="N40" t="inlineStr">
@@ -4828,9 +4859,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="P40" s="40" t="inlineStr">
-        <is>
-          <t>Exam67</t>
+      <c r="P40" s="81" t="inlineStr">
+        <is>
+          <t>Exam70</t>
         </is>
       </c>
       <c r="Q40" t="inlineStr">
@@ -4843,9 +4874,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="S40" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="S40" s="11" t="inlineStr">
+        <is>
+          <t>Exam72</t>
         </is>
       </c>
     </row>
@@ -4870,9 +4901,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="E41" s="1" t="inlineStr">
+        <is>
+          <t>Exam17</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -4982,9 +5013,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="H42" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="H42" s="82" t="inlineStr">
+        <is>
+          <t>Exam31</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
@@ -4997,9 +5028,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="K42" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="K42" s="42" t="inlineStr">
+        <is>
+          <t>Exam51</t>
         </is>
       </c>
       <c r="L42" t="inlineStr">
@@ -5017,9 +5048,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="O42" s="78" t="inlineStr">
-        <is>
-          <t>Exam61</t>
+      <c r="O42" s="30" t="inlineStr">
+        <is>
+          <t>Exam66</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
@@ -5074,9 +5105,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="G43" s="83" t="inlineStr">
+        <is>
+          <t>Exam29</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
@@ -5089,9 +5120,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="J43" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="J43" s="84" t="inlineStr">
+        <is>
+          <t>Exam40</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
@@ -5099,9 +5130,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="L43" s="79" t="inlineStr">
-        <is>
-          <t>Exam54</t>
+      <c r="L43" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="M43" t="inlineStr">
@@ -5109,9 +5140,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="N43" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="N43" s="85" t="inlineStr">
+        <is>
+          <t>Exam58</t>
         </is>
       </c>
       <c r="O43" t="inlineStr">
@@ -5201,9 +5232,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="M44" s="80" t="inlineStr">
-        <is>
-          <t>Exam55</t>
+      <c r="M44" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="N44" t="inlineStr">
@@ -5253,9 +5284,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="D45" s="53" t="inlineStr">
-        <is>
-          <t>Exam14</t>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
@@ -5293,9 +5324,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="L45" s="74" t="inlineStr">
-        <is>
-          <t>Exam52</t>
+      <c r="L45" s="86" t="inlineStr">
+        <is>
+          <t>Exam54</t>
         </is>
       </c>
       <c r="M45" t="inlineStr">
@@ -5328,7 +5359,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="S45" s="9" t="inlineStr">
+      <c r="S45" s="41" t="inlineStr">
         <is>
           <t>Exam74</t>
         </is>
@@ -5360,7 +5391,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="F46" s="81" t="inlineStr">
+      <c r="F46" s="87" t="inlineStr">
         <is>
           <t>Exam25</t>
         </is>
@@ -5462,9 +5493,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="G47" s="88" t="inlineStr">
+        <is>
+          <t>Exam30</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
@@ -5564,9 +5595,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="H48" s="1" t="inlineStr">
-        <is>
-          <t>Exam34</t>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
@@ -5599,7 +5630,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="O48" s="32" t="inlineStr">
+      <c r="O48" s="30" t="inlineStr">
         <is>
           <t>Exam66</t>
         </is>
@@ -5646,9 +5677,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="E49" s="17" t="inlineStr">
-        <is>
-          <t>Exam17</t>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -5666,9 +5697,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="I49" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="I49" s="19" t="inlineStr">
+        <is>
+          <t>Exam35</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
@@ -5691,9 +5722,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="N49" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="N49" s="89" t="inlineStr">
+        <is>
+          <t>Exam59</t>
         </is>
       </c>
       <c r="O49" t="inlineStr">
@@ -5733,9 +5764,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="C50" s="82" t="inlineStr">
-        <is>
-          <t>Exam6</t>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -5748,9 +5779,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="F50" s="10" t="inlineStr">
-        <is>
-          <t>Exam24</t>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
@@ -5758,9 +5789,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="H50" s="54" t="inlineStr">
-        <is>
-          <t>Exam31</t>
+      <c r="H50" s="4" t="inlineStr">
+        <is>
+          <t>Exam34</t>
         </is>
       </c>
       <c r="I50" t="inlineStr">
@@ -5768,9 +5799,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="J50" s="73" t="inlineStr">
-        <is>
-          <t>Exam40</t>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="K50" t="inlineStr">
@@ -5783,9 +5814,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="M50" s="83" t="inlineStr">
-        <is>
-          <t>Exam55</t>
+      <c r="M50" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="N50" t="inlineStr">
@@ -5793,9 +5824,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="O50" s="63" t="inlineStr">
-        <is>
-          <t>Exam62</t>
+      <c r="O50" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
@@ -5813,9 +5844,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="S50" s="9" t="inlineStr">
-        <is>
-          <t>Exam74</t>
+      <c r="S50" s="11" t="inlineStr">
+        <is>
+          <t>Exam72</t>
         </is>
       </c>
     </row>
@@ -5860,9 +5891,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="I51" s="18" t="inlineStr">
-        <is>
-          <t>Exam35</t>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="J51" t="inlineStr">
@@ -5870,9 +5901,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="K51" s="84" t="inlineStr">
-        <is>
-          <t>Exam48</t>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="L51" t="inlineStr">
@@ -5922,9 +5953,9 @@
           <t>Mary Ross</t>
         </is>
       </c>
-      <c r="B52" s="58" t="inlineStr">
-        <is>
-          <t>Exam4</t>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -5932,9 +5963,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="D52" s="90" t="inlineStr">
+        <is>
+          <t>Exam12</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
@@ -5947,7 +5978,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="G52" s="43" t="inlineStr">
+      <c r="G52" s="91" t="inlineStr">
         <is>
           <t>Exam30</t>
         </is>
@@ -5957,9 +5988,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="I52" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="I52" s="92" t="inlineStr">
+        <is>
+          <t>Exam36</t>
         </is>
       </c>
       <c r="J52" t="inlineStr">
@@ -5967,7 +5998,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="K52" s="85" t="inlineStr">
+      <c r="K52" s="93" t="inlineStr">
         <is>
           <t>Exam46</t>
         </is>
@@ -5992,9 +6023,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="P52" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="P52" s="59" t="inlineStr">
+        <is>
+          <t>Exam67</t>
         </is>
       </c>
       <c r="Q52" t="inlineStr">
@@ -6007,9 +6038,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="S52" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="S52" s="41" t="inlineStr">
+        <is>
+          <t>Exam74</t>
         </is>
       </c>
     </row>
@@ -6034,9 +6065,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="E53" s="94" t="inlineStr">
+        <is>
+          <t>Exam16</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -6049,9 +6080,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="H53" s="1" t="inlineStr">
-        <is>
-          <t>Exam34</t>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="I53" t="inlineStr">
@@ -6079,7 +6110,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="N53" s="2" t="inlineStr">
+      <c r="N53" s="85" t="inlineStr">
         <is>
           <t>Exam58</t>
         </is>
@@ -6089,9 +6120,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="P53" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="P53" s="45" t="inlineStr">
+        <is>
+          <t>Exam67</t>
         </is>
       </c>
       <c r="Q53" t="inlineStr">
@@ -6151,9 +6182,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="I54" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="I54" s="95" t="inlineStr">
+        <is>
+          <t>Exam39</t>
         </is>
       </c>
       <c r="J54" t="inlineStr">
@@ -6181,7 +6212,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="O54" s="32" t="inlineStr">
+      <c r="O54" s="30" t="inlineStr">
         <is>
           <t>Exam66</t>
         </is>
@@ -6201,9 +6232,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="S54" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="S54" s="20" t="inlineStr">
+        <is>
+          <t>Exam72</t>
         </is>
       </c>
     </row>
@@ -6213,9 +6244,9 @@
           <t>Nathaniel Foster</t>
         </is>
       </c>
-      <c r="B55" s="75" t="inlineStr">
-        <is>
-          <t>Exam5</t>
+      <c r="B55" s="71" t="inlineStr">
+        <is>
+          <t>Exam3</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -6228,9 +6259,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="E55" s="59" t="inlineStr">
-        <is>
-          <t>Exam17</t>
+      <c r="E55" s="96" t="inlineStr">
+        <is>
+          <t>Exam16</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -6243,9 +6274,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="H55" s="86" t="inlineStr">
-        <is>
-          <t>Exam33</t>
+      <c r="H55" s="38" t="inlineStr">
+        <is>
+          <t>Exam32</t>
         </is>
       </c>
       <c r="I55" t="inlineStr">
@@ -6263,9 +6294,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="L55" s="11" t="inlineStr">
-        <is>
-          <t>Exam53</t>
+      <c r="L55" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="M55" t="inlineStr">
@@ -6273,9 +6304,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="N55" s="87" t="inlineStr">
-        <is>
-          <t>Exam58</t>
+      <c r="N55" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="O55" t="inlineStr">
@@ -6283,14 +6314,14 @@
           <t>-</t>
         </is>
       </c>
-      <c r="P55" s="88" t="inlineStr">
-        <is>
-          <t>Exam69</t>
-        </is>
-      </c>
-      <c r="Q55" s="31" t="inlineStr">
-        <is>
-          <t>Exam72</t>
+      <c r="P55" s="97" t="inlineStr">
+        <is>
+          <t>Exam68</t>
+        </is>
+      </c>
+      <c r="Q55" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="R55" t="inlineStr">
@@ -6298,9 +6329,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="S55" s="9" t="inlineStr">
-        <is>
-          <t>Exam74</t>
+      <c r="S55" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
     </row>
@@ -6330,9 +6361,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="F56" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="F56" s="87" t="inlineStr">
+        <is>
+          <t>Exam25</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
@@ -6355,9 +6386,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="K56" s="89" t="inlineStr">
-        <is>
-          <t>Exam47</t>
+      <c r="K56" s="42" t="inlineStr">
+        <is>
+          <t>Exam51</t>
         </is>
       </c>
       <c r="L56" t="inlineStr">
@@ -6365,9 +6396,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="M56" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="M56" s="98" t="inlineStr">
+        <is>
+          <t>Exam56</t>
         </is>
       </c>
       <c r="N56" t="inlineStr">
@@ -6375,9 +6406,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="O56" s="32" t="inlineStr">
-        <is>
-          <t>Exam66</t>
+      <c r="O56" s="99" t="inlineStr">
+        <is>
+          <t>Exam61</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
@@ -6504,9 +6535,9 @@
           <t>Patrick Foster</t>
         </is>
       </c>
-      <c r="B58" s="90" t="inlineStr">
-        <is>
-          <t>Exam1</t>
+      <c r="B58" s="100" t="inlineStr">
+        <is>
+          <t>Exam2</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -6514,9 +6545,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="D58" s="91" t="inlineStr">
-        <is>
-          <t>Exam11</t>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
@@ -6524,9 +6555,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="F58" s="76" t="inlineStr">
-        <is>
-          <t>Exam23</t>
+      <c r="F58" s="101" t="inlineStr">
+        <is>
+          <t>Exam21</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
@@ -6534,9 +6565,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="H58" s="86" t="inlineStr">
-        <is>
-          <t>Exam33</t>
+      <c r="H58" s="4" t="inlineStr">
+        <is>
+          <t>Exam34</t>
         </is>
       </c>
       <c r="I58" t="inlineStr">
@@ -6574,9 +6605,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="P58" s="40" t="inlineStr">
-        <is>
-          <t>Exam67</t>
+      <c r="P58" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="Q58" t="inlineStr">
@@ -6589,9 +6620,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="S58" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="S58" s="11" t="inlineStr">
+        <is>
+          <t>Exam72</t>
         </is>
       </c>
     </row>
@@ -6626,9 +6657,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="G59" s="42" t="inlineStr">
-        <is>
-          <t>Exam28</t>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
@@ -6636,9 +6667,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="I59" s="18" t="inlineStr">
-        <is>
-          <t>Exam35</t>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="J59" t="inlineStr">
@@ -6661,9 +6692,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="N59" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="N59" s="102" t="inlineStr">
+        <is>
+          <t>Exam60</t>
         </is>
       </c>
       <c r="O59" t="inlineStr">
@@ -6671,9 +6702,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="P59" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="P59" s="103" t="inlineStr">
+        <is>
+          <t>Exam68</t>
         </is>
       </c>
       <c r="Q59" t="inlineStr">
@@ -6728,9 +6759,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="H60" s="1" t="inlineStr">
-        <is>
-          <t>Exam34</t>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="I60" t="inlineStr">
@@ -6738,9 +6769,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="J60" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="J60" s="104" t="inlineStr">
+        <is>
+          <t>Exam42</t>
         </is>
       </c>
       <c r="K60" t="inlineStr">
@@ -6763,7 +6794,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="O60" s="32" t="inlineStr">
+      <c r="O60" s="30" t="inlineStr">
         <is>
           <t>Exam66</t>
         </is>
@@ -6795,9 +6826,9 @@
           <t>Rachel Hughes</t>
         </is>
       </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="B61" s="31" t="inlineStr">
+        <is>
+          <t>Exam4</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -6810,9 +6841,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="E61" s="17" t="inlineStr">
-        <is>
-          <t>Exam17</t>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -6820,9 +6851,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="G61" s="42" t="inlineStr">
-        <is>
-          <t>Exam28</t>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
@@ -6840,9 +6871,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="K61" s="92" t="inlineStr">
-        <is>
-          <t>Exam50</t>
+      <c r="K61" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="L61" t="inlineStr">
@@ -6850,9 +6881,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="M61" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="M61" s="98" t="inlineStr">
+        <is>
+          <t>Exam56</t>
         </is>
       </c>
       <c r="N61" t="inlineStr">
@@ -6865,9 +6896,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="P61" s="47" t="inlineStr">
-        <is>
-          <t>Exam67</t>
+      <c r="P61" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="Q61" t="inlineStr">
@@ -6897,9 +6928,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="C62" s="93" t="inlineStr">
-        <is>
-          <t>Exam9</t>
+      <c r="C62" s="105" t="inlineStr">
+        <is>
+          <t>Exam7</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -6912,9 +6943,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="F62" s="94" t="inlineStr">
-        <is>
-          <t>Exam22</t>
+      <c r="F62" s="106" t="inlineStr">
+        <is>
+          <t>Exam23</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
@@ -6922,9 +6953,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="H62" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="H62" s="107" t="inlineStr">
+        <is>
+          <t>Exam33</t>
         </is>
       </c>
       <c r="I62" t="inlineStr">
@@ -6952,9 +6983,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="N62" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="N62" s="108" t="inlineStr">
+        <is>
+          <t>Exam59</t>
         </is>
       </c>
       <c r="O62" t="inlineStr">
@@ -6962,9 +6993,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="P62" s="88" t="inlineStr">
-        <is>
-          <t>Exam69</t>
+      <c r="P62" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="Q62" t="inlineStr">
@@ -6999,9 +7030,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="D63" s="95" t="inlineStr">
-        <is>
-          <t>Exam15</t>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
@@ -7024,9 +7055,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="I63" s="18" t="inlineStr">
-        <is>
-          <t>Exam35</t>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="J63" t="inlineStr">
@@ -7034,9 +7065,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="K63" s="20" t="inlineStr">
-        <is>
-          <t>Exam51</t>
+      <c r="K63" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="L63" t="inlineStr">
@@ -7054,9 +7085,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="O63" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="O63" s="109" t="inlineStr">
+        <is>
+          <t>Exam63</t>
         </is>
       </c>
       <c r="P63" t="inlineStr">
@@ -7074,9 +7105,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="S63" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="S63" s="20" t="inlineStr">
+        <is>
+          <t>Exam72</t>
         </is>
       </c>
     </row>
@@ -7086,9 +7117,9 @@
           <t>Robert Price</t>
         </is>
       </c>
-      <c r="B64" s="52" t="inlineStr">
-        <is>
-          <t>Exam3</t>
+      <c r="B64" s="110" t="inlineStr">
+        <is>
+          <t>Exam1</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -7111,7 +7142,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="G64" s="60" t="inlineStr">
+      <c r="G64" s="111" t="inlineStr">
         <is>
           <t>Exam26</t>
         </is>
@@ -7121,9 +7152,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="I64" s="96" t="inlineStr">
-        <is>
-          <t>Exam38</t>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="J64" t="inlineStr">
@@ -7131,9 +7162,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="K64" s="97" t="inlineStr">
-        <is>
-          <t>Exam45</t>
+      <c r="K64" s="112" t="inlineStr">
+        <is>
+          <t>Exam50</t>
         </is>
       </c>
       <c r="L64" t="inlineStr">
@@ -7141,9 +7172,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="M64" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="M64" s="113" t="inlineStr">
+        <is>
+          <t>Exam55</t>
         </is>
       </c>
       <c r="N64" t="inlineStr">
@@ -7156,9 +7187,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="P64" s="40" t="inlineStr">
-        <is>
-          <t>Exam67</t>
+      <c r="P64" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="Q64" t="inlineStr">
@@ -7171,9 +7202,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="S64" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="S64" s="41" t="inlineStr">
+        <is>
+          <t>Exam74</t>
         </is>
       </c>
     </row>
@@ -7188,9 +7219,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="C65" s="98" t="inlineStr">
-        <is>
-          <t>Exam8</t>
+      <c r="C65" s="114" t="inlineStr">
+        <is>
+          <t>Exam6</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -7198,9 +7229,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="E65" s="99" t="inlineStr">
-        <is>
-          <t>Exam20</t>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -7213,9 +7244,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="H65" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="H65" s="4" t="inlineStr">
+        <is>
+          <t>Exam34</t>
         </is>
       </c>
       <c r="I65" t="inlineStr">
@@ -7243,9 +7274,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="N65" s="100" t="inlineStr">
-        <is>
-          <t>Exam60</t>
+      <c r="N65" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="O65" t="inlineStr">
@@ -7258,9 +7289,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="Q65" s="31" t="inlineStr">
-        <is>
-          <t>Exam72</t>
+      <c r="Q65" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="R65" t="inlineStr">
@@ -7268,9 +7299,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="S65" s="64" t="inlineStr">
-        <is>
-          <t>Exam73</t>
+      <c r="S65" s="7" t="inlineStr">
+        <is>
+          <t>Exam75</t>
         </is>
       </c>
     </row>
@@ -7345,9 +7376,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="O66" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="O66" s="115" t="inlineStr">
+        <is>
+          <t>Exam65</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
@@ -7365,9 +7396,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="S66" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="S66" s="20" t="inlineStr">
+        <is>
+          <t>Exam72</t>
         </is>
       </c>
     </row>
@@ -7377,9 +7408,9 @@
           <t>Sarah Cox</t>
         </is>
       </c>
-      <c r="B67" s="16" t="inlineStr">
-        <is>
-          <t>Exam4</t>
+      <c r="B67" s="116" t="inlineStr">
+        <is>
+          <t>Exam2</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -7519,9 +7550,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="K68" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="K68" s="117" t="inlineStr">
+        <is>
+          <t>Exam47</t>
         </is>
       </c>
       <c r="L68" t="inlineStr">
@@ -7539,9 +7570,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="O68" s="32" t="inlineStr">
-        <is>
-          <t>Exam66</t>
+      <c r="O68" s="118" t="inlineStr">
+        <is>
+          <t>Exam64</t>
         </is>
       </c>
       <c r="P68" t="inlineStr">
@@ -7581,9 +7612,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="D69" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="D69" s="119" t="inlineStr">
+        <is>
+          <t>Exam13</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
@@ -7631,9 +7662,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="N69" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="N69" s="50" t="inlineStr">
+        <is>
+          <t>Exam57</t>
         </is>
       </c>
       <c r="O69" t="inlineStr">
@@ -7646,9 +7677,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="Q69" s="3" t="inlineStr">
-        <is>
-          <t>Exam72</t>
+      <c r="Q69" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="R69" t="inlineStr">
@@ -7656,7 +7687,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="S69" t="inlineStr">
+      <c r="S69" s="44" t="inlineStr">
         <is>
           <t>Exam74</t>
         </is>
@@ -7703,9 +7734,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="I70" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="I70" s="19" t="inlineStr">
+        <is>
+          <t>Exam35</t>
         </is>
       </c>
       <c r="J70" t="inlineStr">
@@ -7713,9 +7744,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="K70" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="K70" s="120" t="inlineStr">
+        <is>
+          <t>Exam50</t>
         </is>
       </c>
       <c r="L70" t="inlineStr">
@@ -7738,9 +7769,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="P70" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="P70" s="45" t="inlineStr">
+        <is>
+          <t>Exam67</t>
         </is>
       </c>
       <c r="Q70" t="inlineStr">
@@ -7753,9 +7784,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="S70" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="S70" s="20" t="inlineStr">
+        <is>
+          <t>Exam72</t>
         </is>
       </c>
     </row>
@@ -7780,9 +7811,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="E71" s="101" t="inlineStr">
-        <is>
-          <t>Exam16</t>
+      <c r="E71" s="1" t="inlineStr">
+        <is>
+          <t>Exam17</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -7815,9 +7846,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="L71" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="L71" s="121" t="inlineStr">
+        <is>
+          <t>Exam52</t>
         </is>
       </c>
       <c r="M71" t="inlineStr">
@@ -7872,9 +7903,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="D72" s="26" t="inlineStr">
-        <is>
-          <t>Exam13</t>
+      <c r="D72" s="90" t="inlineStr">
+        <is>
+          <t>Exam12</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
@@ -7892,9 +7923,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="H72" s="70" t="inlineStr">
-        <is>
-          <t>Exam32</t>
+      <c r="H72" s="4" t="inlineStr">
+        <is>
+          <t>Exam34</t>
         </is>
       </c>
       <c r="I72" t="inlineStr">
@@ -7907,9 +7938,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="K72" s="102" t="inlineStr">
-        <is>
-          <t>Exam47</t>
+      <c r="K72" s="122" t="inlineStr">
+        <is>
+          <t>Exam43</t>
         </is>
       </c>
       <c r="L72" t="inlineStr">
@@ -7917,9 +7948,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="M72" s="29" t="inlineStr">
-        <is>
-          <t>Exam56</t>
+      <c r="M72" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="N72" t="inlineStr">
@@ -7927,9 +7958,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="O72" s="103" t="inlineStr">
-        <is>
-          <t>Exam65</t>
+      <c r="O72" s="123" t="inlineStr">
+        <is>
+          <t>Exam62</t>
         </is>
       </c>
       <c r="P72" t="inlineStr">
@@ -7947,9 +7978,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="S72" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="S72" s="15" t="inlineStr">
+        <is>
+          <t>Exam73</t>
         </is>
       </c>
     </row>
@@ -7959,9 +7990,9 @@
           <t>Walter Gray</t>
         </is>
       </c>
-      <c r="B73" s="104" t="inlineStr">
-        <is>
-          <t>Exam2</t>
+      <c r="B73" s="31" t="inlineStr">
+        <is>
+          <t>Exam4</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -8061,9 +8092,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="C74" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="C74" s="16" t="inlineStr">
+        <is>
+          <t>Exam6</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -8076,9 +8107,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="F74" s="81" t="inlineStr">
-        <is>
-          <t>Exam25</t>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
@@ -8086,9 +8117,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="H74" s="1" t="inlineStr">
-        <is>
-          <t>Exam34</t>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="I74" t="inlineStr">
@@ -8101,9 +8132,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="K74" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="K74" s="124" t="inlineStr">
+        <is>
+          <t>Exam49</t>
         </is>
       </c>
       <c r="L74" t="inlineStr">
@@ -8121,7 +8152,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="O74" s="32" t="inlineStr">
+      <c r="O74" s="30" t="inlineStr">
         <is>
           <t>Exam66</t>
         </is>
@@ -8178,9 +8209,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="G75" s="105" t="inlineStr">
-        <is>
-          <t>Exam29</t>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="H75" t="inlineStr">
@@ -8188,9 +8219,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="I75" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="I75" s="19" t="inlineStr">
+        <is>
+          <t>Exam35</t>
         </is>
       </c>
       <c r="J75" t="inlineStr">
@@ -8203,9 +8234,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="L75" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="L75" s="125" t="inlineStr">
+        <is>
+          <t>Exam54</t>
         </is>
       </c>
       <c r="M75" t="inlineStr">
@@ -8213,9 +8244,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="N75" s="106" t="inlineStr">
-        <is>
-          <t>Exam57</t>
+      <c r="N75" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="O75" t="inlineStr">
@@ -8228,9 +8259,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="Q75" s="107" t="inlineStr">
-        <is>
-          <t>Exam71</t>
+      <c r="Q75" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
       <c r="R75" t="inlineStr">
@@ -8238,7 +8269,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="S75" t="inlineStr">
+      <c r="S75" s="44" t="inlineStr">
         <is>
           <t>Exam74</t>
         </is>
@@ -8250,9 +8281,9 @@
           <t>Zachary Brooks</t>
         </is>
       </c>
-      <c r="B76" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="B76" s="126" t="inlineStr">
+        <is>
+          <t>Exam3</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -8280,7 +8311,7 @@
           <t>-</t>
         </is>
       </c>
-      <c r="H76" s="1" t="inlineStr">
+      <c r="H76" s="17" t="inlineStr">
         <is>
           <t>Exam34</t>
         </is>
@@ -8320,9 +8351,9 @@
           <t>-</t>
         </is>
       </c>
-      <c r="P76" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="P76" s="45" t="inlineStr">
+        <is>
+          <t>Exam67</t>
         </is>
       </c>
       <c r="Q76" t="inlineStr">

</xml_diff>